<commit_message>
PIN-2249: Income level changed to income
</commit_message>
<xml_diff>
--- a/tests/NewApiBundle/Resources/KHM-Import-1HH-0HHM-0HHM-excel-date-format.xlsx
+++ b/tests/NewApiBundle/Resources/KHM-Import-1HH-0HHM-0HHM-excel-date-format.xlsx
@@ -41,7 +41,7 @@
     <t xml:space="preserve">Livelihood</t>
   </si>
   <si>
-    <t xml:space="preserve">Income level</t>
+    <t xml:space="preserve">Income</t>
   </si>
   <si>
     <t xml:space="preserve">Food Consumption Score</t>
@@ -576,10 +576,10 @@
   <dimension ref="A1:BG1007"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.4"/>
@@ -3349,7 +3349,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.7"/>
   </cols>

</xml_diff>